<commit_message>
add publication request descr 7a1a9b4308042effab877c2ea087f4459ae968cc
</commit_message>
<xml_diff>
--- a/ig/nr/correctErrors/StructureDefinition-PDSmintendedrecipient.xlsx
+++ b/ig/nr/correctErrors/StructureDefinition-PDSmintendedrecipient.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>3.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-20T10:49:37+00:00</t>
+    <t>2023-03-20T10:53:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>